<commit_message>
dont know what caused changes here
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_RES_APP_EffProj.xlsx
+++ b/SuppXLS/Scen_RES_APP_EffProj.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\TIMES-DK_COMETS_new\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TIMES models\TIMES-tom\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDDAB49-0971-4BFF-B9FB-90361E558BC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFE46D4-639E-4AEE-95F2-E28DC6F653D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="2880" windowWidth="21555" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16008" yWindow="1212" windowWidth="21012" windowHeight="14256" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LOG" sheetId="24" r:id="rId1"/>
@@ -36,7 +36,10 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -9264,13 +9267,13 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="4" max="4" width="19.88671875" customWidth="1"/>
+    <col min="5" max="5" width="60.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5">
@@ -9321,20 +9324,20 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="61"/>
+    <col min="1" max="1" width="9.109375" style="61"/>
     <col min="2" max="2" width="24" style="61" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="138.42578125" style="61" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="61"/>
+    <col min="3" max="3" width="138.44140625" style="61" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="18.75">
+    <row r="1" spans="2:3" ht="18">
       <c r="B1" s="60" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="15">
+    <row r="3" spans="2:3" ht="14.4">
       <c r="B3" s="62" t="s">
         <v>120</v>
       </c>
@@ -9342,7 +9345,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="15">
+    <row r="4" spans="2:3" ht="14.4">
       <c r="B4" s="62" t="s">
         <v>121</v>
       </c>
@@ -9350,10 +9353,10 @@
         <v>138</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="15">
+    <row r="5" spans="2:3" ht="14.4">
       <c r="B5" s="62"/>
     </row>
-    <row r="6" spans="2:3" ht="15">
+    <row r="6" spans="2:3" ht="14.4">
       <c r="B6" s="62" t="s">
         <v>122</v>
       </c>
@@ -9361,15 +9364,15 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="15">
+    <row r="7" spans="2:3" ht="14.4">
       <c r="B7" s="62"/>
     </row>
-    <row r="8" spans="2:3" ht="15">
+    <row r="8" spans="2:3" ht="14.4">
       <c r="B8" s="63" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="15">
+    <row r="9" spans="2:3" ht="14.4">
       <c r="B9" s="62"/>
     </row>
     <row r="10" spans="2:3">
@@ -9380,7 +9383,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="15">
+    <row r="11" spans="2:3" ht="14.4">
       <c r="B11" s="64" t="s">
         <v>131</v>
       </c>
@@ -9388,7 +9391,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15">
+    <row r="12" spans="2:3" ht="14.4">
       <c r="B12" s="64" t="s">
         <v>132</v>
       </c>
@@ -9437,11 +9440,11 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="2" max="2" width="27.42578125" customWidth="1"/>
-    <col min="5" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.44140625" customWidth="1"/>
+    <col min="5" max="6" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
@@ -9450,7 +9453,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:12" ht="13.5" thickBot="1">
+    <row r="3" spans="2:12" ht="13.8" thickBot="1">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -9962,24 +9965,24 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" style="46" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.88671875" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" style="46" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="46"/>
-    <col min="14" max="14" width="9.85546875" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="46"/>
+    <col min="14" max="14" width="9.88671875" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9994,7 +9997,7 @@
         <v>EFF Improvments</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="13.5" thickBot="1">
+    <row r="4" spans="2:16" ht="13.8" thickBot="1">
       <c r="B4" s="3" t="s">
         <v>139</v>
       </c>
@@ -10022,7 +10025,7 @@
       </c>
       <c r="K4" s="24"/>
     </row>
-    <row r="5" spans="2:16" ht="15.75" thickBot="1">
+    <row r="5" spans="2:16" ht="15" thickBot="1">
       <c r="D5" t="s">
         <v>22</v>
       </c>
@@ -10051,7 +10054,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="13.5" thickBot="1">
+    <row r="6" spans="2:16" ht="13.8" thickBot="1">
       <c r="D6" t="s">
         <v>22</v>
       </c>
@@ -10169,7 +10172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="15">
+    <row r="11" spans="2:16" ht="14.4">
       <c r="D11" t="s">
         <v>22</v>
       </c>
@@ -10264,7 +10267,7 @@
         <v>1.1738661511728654</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="15">
+    <row r="15" spans="2:16" ht="14.4">
       <c r="D15" t="s">
         <v>22</v>
       </c>
@@ -10382,7 +10385,7 @@
         <v>1.4030444785119536</v>
       </c>
     </row>
-    <row r="20" spans="4:13" ht="15">
+    <row r="20" spans="4:13" ht="14.4">
       <c r="D20" t="s">
         <v>22</v>
       </c>
@@ -10500,7 +10503,7 @@
         <v>1.9012411315334643</v>
       </c>
     </row>
-    <row r="25" spans="4:13" ht="15">
+    <row r="25" spans="4:13" ht="14.4">
       <c r="D25" t="s">
         <v>22</v>
       </c>
@@ -10618,7 +10621,7 @@
         <v>3.9433699620168672</v>
       </c>
     </row>
-    <row r="30" spans="4:13" ht="15">
+    <row r="30" spans="4:13" ht="14.4">
       <c r="D30" t="s">
         <v>22</v>
       </c>
@@ -10736,7 +10739,7 @@
         <v>1.5038992517729026</v>
       </c>
     </row>
-    <row r="35" spans="4:16" ht="15">
+    <row r="35" spans="4:16" ht="14.4">
       <c r="D35" t="s">
         <v>22</v>
       </c>
@@ -10888,22 +10891,22 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="71" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" style="71" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
-    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" customWidth="1"/>
+    <col min="13" max="13" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10917,7 +10920,7 @@
         <v>EFF Improvments</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="13.5" thickBot="1">
+    <row r="4" spans="2:11" ht="13.8" thickBot="1">
       <c r="B4" s="3" t="s">
         <v>2</v>
       </c>
@@ -10938,7 +10941,7 @@
         <v>Multistorey building</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="15">
+    <row r="5" spans="2:11" ht="14.4">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -11079,7 +11082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="15">
+    <row r="11" spans="2:11" ht="14.4">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -11174,7 +11177,7 @@
         <v>1.1843424286076993</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="15">
+    <row r="15" spans="2:11" ht="14.4">
       <c r="B15" t="s">
         <v>22</v>
       </c>
@@ -11292,7 +11295,7 @@
         <v>1.6766474763468822</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="15">
+    <row r="20" spans="2:11" ht="14.4">
       <c r="B20" t="s">
         <v>22</v>
       </c>
@@ -11415,7 +11418,7 @@
         <v>1.9364140125242728</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="15">
+    <row r="25" spans="2:11" ht="14.4">
       <c r="B25" t="s">
         <v>22</v>
       </c>
@@ -11534,7 +11537,7 @@
         <v>3.9433699620168672</v>
       </c>
     </row>
-    <row r="30" spans="2:11" ht="15">
+    <row r="30" spans="2:11" ht="14.4">
       <c r="B30" t="s">
         <v>22</v>
       </c>
@@ -11652,7 +11655,7 @@
         <v>1.4716104531335674</v>
       </c>
     </row>
-    <row r="35" spans="2:11" ht="15">
+    <row r="35" spans="2:11" ht="14.4">
       <c r="B35" t="s">
         <v>22</v>
       </c>
@@ -11803,10 +11806,10 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="54.42578125" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -11865,7 +11868,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="25.5">
+    <row r="5" spans="1:17" ht="27.6">
       <c r="A5" s="13" t="s">
         <v>39</v>
       </c>
@@ -11915,7 +11918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="13.5" thickBot="1">
+    <row r="6" spans="1:17" ht="13.8" thickBot="1">
       <c r="A6" s="15" t="s">
         <v>51</v>
       </c>
@@ -12376,7 +12379,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="25.5">
+    <row r="23" spans="1:17" ht="27.6">
       <c r="A23" s="13" t="s">
         <v>39</v>
       </c>
@@ -12426,7 +12429,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="13.5" thickBot="1">
+    <row r="24" spans="1:17" ht="13.8" thickBot="1">
       <c r="A24" s="15" t="s">
         <v>51</v>
       </c>
@@ -12874,20 +12877,20 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="28" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" style="28" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="28" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" style="28" customWidth="1"/>
+    <col min="2" max="2" width="6.88671875" style="28" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" style="28" customWidth="1"/>
+    <col min="4" max="4" width="8.109375" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="28"/>
-    <col min="9" max="9" width="9.85546875" style="28" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" style="28" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="9.109375" style="28"/>
+    <col min="9" max="9" width="9.88671875" style="28" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" style="28" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="28" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="28" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="28"/>
+    <col min="13" max="13" width="17.6640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.109375" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:16">
@@ -12911,7 +12914,7 @@
     <row r="3" spans="3:16">
       <c r="C3" s="29"/>
     </row>
-    <row r="4" spans="3:16" ht="13.5" thickBot="1">
+    <row r="4" spans="3:16" ht="13.8" thickBot="1">
       <c r="C4" s="31" t="s">
         <v>4</v>
       </c>
@@ -12934,7 +12937,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="3:16" ht="15">
+    <row r="6" spans="3:16" ht="14.4">
       <c r="C6" s="36" t="s">
         <v>73</v>
       </c>
@@ -12957,7 +12960,7 @@
       <c r="M6" s="39"/>
       <c r="N6" s="39"/>
     </row>
-    <row r="7" spans="3:16" ht="15">
+    <row r="7" spans="3:16" ht="14.4">
       <c r="C7" s="36" t="s">
         <v>73</v>
       </c>
@@ -12980,7 +12983,7 @@
       <c r="M7" s="39"/>
       <c r="N7" s="39"/>
     </row>
-    <row r="8" spans="3:16" ht="15">
+    <row r="8" spans="3:16" ht="14.4">
       <c r="C8" s="36" t="s">
         <v>73</v>
       </c>
@@ -13015,7 +13018,7 @@
       </c>
       <c r="P8" s="39"/>
     </row>
-    <row r="9" spans="3:16" ht="15">
+    <row r="9" spans="3:16" ht="14.4">
       <c r="C9" s="36" t="s">
         <v>73</v>
       </c>
@@ -13050,7 +13053,7 @@
       </c>
       <c r="P9" s="42"/>
     </row>
-    <row r="10" spans="3:16" ht="15">
+    <row r="10" spans="3:16" ht="14.4">
       <c r="C10" s="36" t="s">
         <v>73</v>
       </c>
@@ -13085,7 +13088,7 @@
       </c>
       <c r="P10" s="42"/>
     </row>
-    <row r="11" spans="3:16" ht="15">
+    <row r="11" spans="3:16" ht="14.4">
       <c r="C11" s="36" t="s">
         <v>74</v>
       </c>
@@ -13120,7 +13123,7 @@
       </c>
       <c r="P11" s="42"/>
     </row>
-    <row r="12" spans="3:16" ht="15">
+    <row r="12" spans="3:16" ht="14.4">
       <c r="C12" s="36" t="s">
         <v>74</v>
       </c>
@@ -13155,7 +13158,7 @@
       </c>
       <c r="P12" s="42"/>
     </row>
-    <row r="13" spans="3:16" ht="15">
+    <row r="13" spans="3:16" ht="14.4">
       <c r="C13" s="36" t="s">
         <v>74</v>
       </c>
@@ -13190,7 +13193,7 @@
       </c>
       <c r="P13" s="42"/>
     </row>
-    <row r="14" spans="3:16" ht="15">
+    <row r="14" spans="3:16" ht="14.4">
       <c r="C14" s="36" t="s">
         <v>74</v>
       </c>
@@ -13225,7 +13228,7 @@
       </c>
       <c r="P14" s="42"/>
     </row>
-    <row r="15" spans="3:16" ht="15">
+    <row r="15" spans="3:16" ht="14.4">
       <c r="C15" s="36" t="s">
         <v>74</v>
       </c>
@@ -13348,7 +13351,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="3:20" ht="15">
+    <row r="21" spans="3:20" ht="14.4">
       <c r="C21" s="36" t="s">
         <v>76</v>
       </c>
@@ -13385,7 +13388,7 @@
       <c r="R21" s="39"/>
       <c r="T21" s="39"/>
     </row>
-    <row r="22" spans="3:20" ht="15">
+    <row r="22" spans="3:20" ht="14.4">
       <c r="C22" s="36" t="s">
         <v>76</v>
       </c>
@@ -13422,7 +13425,7 @@
       <c r="R22" s="42"/>
       <c r="T22" s="42"/>
     </row>
-    <row r="23" spans="3:20" ht="15">
+    <row r="23" spans="3:20" ht="14.4">
       <c r="C23" s="36" t="s">
         <v>76</v>
       </c>
@@ -13459,7 +13462,7 @@
       <c r="R23" s="42"/>
       <c r="T23" s="42"/>
     </row>
-    <row r="24" spans="3:20" ht="15">
+    <row r="24" spans="3:20" ht="14.4">
       <c r="C24" s="36" t="s">
         <v>76</v>
       </c>
@@ -13496,7 +13499,7 @@
       <c r="R24" s="42"/>
       <c r="T24" s="42"/>
     </row>
-    <row r="25" spans="3:20" ht="15">
+    <row r="25" spans="3:20" ht="14.4">
       <c r="C25" s="36" t="s">
         <v>76</v>
       </c>
@@ -13533,7 +13536,7 @@
       <c r="R25" s="42"/>
       <c r="T25" s="42"/>
     </row>
-    <row r="26" spans="3:20" ht="15">
+    <row r="26" spans="3:20" ht="14.4">
       <c r="C26" s="36" t="s">
         <v>77</v>
       </c>
@@ -13570,7 +13573,7 @@
       <c r="R26" s="42"/>
       <c r="T26" s="42"/>
     </row>
-    <row r="27" spans="3:20" ht="15">
+    <row r="27" spans="3:20" ht="14.4">
       <c r="C27" s="36" t="s">
         <v>77</v>
       </c>
@@ -13607,7 +13610,7 @@
       <c r="R27" s="42"/>
       <c r="T27" s="42"/>
     </row>
-    <row r="28" spans="3:20" ht="15">
+    <row r="28" spans="3:20" ht="14.4">
       <c r="C28" s="36" t="s">
         <v>77</v>
       </c>

</xml_diff>